<commit_message>
Novos códigos de retorno
</commit_message>
<xml_diff>
--- a/documentacao/frota_coderros_autorizador.xlsx
+++ b/documentacao/frota_coderros_autorizador.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t xml:space="preserve">Transação de Combustível Veículo</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t xml:space="preserve">Equipamento informado não tem vínculo com o Funcionário informado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transação de Serviços</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produtos inválidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Códigos de Produtos informados não encontrados na base ou Produtos não vinculados ao Estabelecimentos</t>
   </si>
 </sst>
 </file>
@@ -308,9 +317,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -346,50 +359,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="80.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -400,7 +413,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -411,7 +424,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -422,7 +435,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -433,7 +446,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -444,7 +457,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -455,7 +468,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -466,7 +479,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -477,7 +490,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -488,7 +501,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -499,7 +512,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -510,7 +523,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -521,7 +534,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -532,7 +545,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -543,7 +556,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -554,7 +567,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -564,8 +577,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -576,7 +589,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -586,25 +599,25 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="0" t="s">
@@ -615,7 +628,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="0" t="s">
@@ -625,12 +638,28 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Limite em Empresa & Atualização de Saldo & Transação Cancelamento
</commit_message>
<xml_diff>
--- a/documentacao/frota_coderros_autorizador.xlsx
+++ b/documentacao/frota_coderros_autorizador.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t xml:space="preserve">Transação de Combustível Veículo</t>
   </si>
@@ -205,6 +205,42 @@
   </si>
   <si>
     <t xml:space="preserve">Senha informada não confere com a senha do cartão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervalo de Tempo inválido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentativa de novo abastecimento realizada em um intervalo de tempo inferior ao mínimo permitido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervalo Percorrido inválido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentativa de novo abastecimento realizada em um intervalo de kms percorridos inferior ao mínimo permitido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horário inválido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentativa de abastecimento fora do horário permitido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qtde litros abastecidos inválida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentativa de abastecimento acima da litragem máxima permitida</t>
   </si>
   <si>
     <t xml:space="preserve">Transação de Combustível Equipamento</t>
@@ -359,17 +395,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="80.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="88.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -600,66 +636,110 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="2"/>
+      <c r="A23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>2</v>
+      <c r="A24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>67</v>
-      </c>
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="2"/>
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>70</v>
+      <c r="B33" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Hibernate Filter + Relatórios + Correções
</commit_message>
<xml_diff>
--- a/documentacao/frota_coderros_autorizador.xlsx
+++ b/documentacao/frota_coderros_autorizador.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t xml:space="preserve">Transação de Combustível Veículo</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t xml:space="preserve">Tentativa de abastecimento acima da litragem máxima permitida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia semana inválido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentativa de abastecimento em um dia de semana não permitido</t>
   </si>
   <si>
     <t xml:space="preserve">Transação de Combustível Equipamento</t>
@@ -395,10 +404,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -680,31 +689,31 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="2"/>
+      <c r="A27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,28 +727,39 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B31" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>82</v>
+      <c r="B34" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>